<commit_message>
1. Real time upload supported for multiple table. 2. Entity Definitions table imported for automating table sync
</commit_message>
<xml_diff>
--- a/ExcelWebAddIn_CWeb/SupportDocs/table sync logic.xlsx
+++ b/ExcelWebAddIn_CWeb/SupportDocs/table sync logic.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K149482\source\repos\ExcelWebAddIn_C\ExcelWebAddIn_CWeb\SupportDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0A462A-940E-4F95-9042-DA46D08C3DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA7E1A5-BB88-4E8F-A817-876A6F156829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{DBCB1CE0-D54F-472B-9A12-147544FDA472}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{DBCB1CE0-D54F-472B-9A12-147544FDA472}"/>
   </bookViews>
   <sheets>
     <sheet name="sync logic in symbol" sheetId="1" r:id="rId1"/>
     <sheet name="mapping logic" sheetId="2" r:id="rId2"/>
+    <sheet name="Refresh Logic when open" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
   <si>
     <t>Change Type</t>
   </si>
@@ -477,6 +478,18 @@
   </si>
   <si>
     <t>use customised order to do the sort</t>
+  </si>
+  <si>
+    <t>loop through all table in the workbook</t>
+  </si>
+  <si>
+    <t>find the valid ones</t>
+  </si>
+  <si>
+    <t>build odata query based on the valid fields (convert eacb to P+)</t>
+  </si>
+  <si>
+    <t>allow gap field</t>
   </si>
 </sst>
 </file>
@@ -879,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -921,20 +934,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -943,8 +956,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2905,8 +2916,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2978,13 +2989,13 @@
       <c r="A4" s="44">
         <v>3</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -3044,7 +3055,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="50" t="s">
+      <c r="B12" t="s">
         <v>120</v>
       </c>
       <c r="C12" t="s">
@@ -3052,7 +3063,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="50" t="s">
+      <c r="B13" t="s">
         <v>121</v>
       </c>
       <c r="C13" t="s">
@@ -3106,7 +3117,7 @@
       <c r="B21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F21" s="51" t="s">
+      <c r="F21" s="49" t="s">
         <v>80</v>
       </c>
       <c r="J21" s="10" t="s">
@@ -3388,7 +3399,7 @@
       <c r="F45" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="G45" s="52"/>
+      <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
@@ -3413,4 +3424,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C39AF8-29E6-4DDC-B233-9FAC254258F2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1. True workbook id added 2. lookup info retrieved
</commit_message>
<xml_diff>
--- a/ExcelWebAddIn_CWeb/SupportDocs/table sync logic.xlsx
+++ b/ExcelWebAddIn_CWeb/SupportDocs/table sync logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K149482\source\repos\ExcelWebAddIn_C\ExcelWebAddIn_CWeb\SupportDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0278C4-785A-474C-B03B-1B15D667242D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90799619-6C99-48FD-A90C-7D6614773EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{DBCB1CE0-D54F-472B-9A12-147544FDA472}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="152">
   <si>
     <t>Change Type</t>
   </si>
@@ -468,9 +468,6 @@
     <t>Table Logical Name</t>
   </si>
   <si>
-    <t>Table Hash Value</t>
-  </si>
-  <si>
     <t>if change, then not equal to the hash value.</t>
   </si>
   <si>
@@ -499,6 +496,12 @@
   </si>
   <si>
     <t>ABBA - if paste whole col as formula</t>
+  </si>
+  <si>
+    <t>Row Hash Value</t>
+  </si>
+  <si>
+    <t>Workbook GUID</t>
   </si>
 </sst>
 </file>
@@ -901,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -967,9 +970,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2915,25 +2915,25 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2948,8 +2948,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3415,35 +3415,48 @@
         <v>136</v>
       </c>
     </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+    </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="G45" s="50"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
-      <c r="G46" s="11"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G48" s="11"/>
     </row>
@@ -3469,22 +3482,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>